<commit_message>
QTM & several changes (agents, plots, source)
- a few new RubiksCube agents
- new plots w.r.t. RubiksCube
- bug fix in LogManagerGUI: correct load of RubiksCube logs
- switch to "HTM" and "QTM" instead of "ALL" and "QUARTER"
- new DAVI4Agent (autodidactic, still experimental)
- made QTM work (bug fix in GameBoardCubeGui)
- extended MCTSWrapperAgentTest to QTM
- new test DAVI_Test
</commit_message>
<xml_diff>
--- a/agents/RubiksCube/2x2x2_STICKER2_AT/csv/mRubiks2x2-MWrap(TCL4-p13)-SoftMax-p1-13-EE20.xlsx
+++ b/agents/RubiksCube/2x2x2_STICKER2_AT/csv/mRubiks2x2-MWrap(TCL4-p13)-SoftMax-p1-13-EE20.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolfgang\Documents\GitHub\GBG\agents\RubiksCube\2x2x2_STICKER2_AT\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04E4AB3B-0479-455C-9194-52A35FF36618}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638D8008-C7F1-40A9-8853-C7DF303687A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="8544"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="8544" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mRubiks2x2-MWrap(TCL4-p13)-Soft" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'mRubiks2x2-MWrap(TCL4-p13)-Soft'!$A$3:$K$3</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -67,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -902,11 +905,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A315"/>
+      <selection activeCell="A3" sqref="A3:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11877,6 +11880,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:K3" xr:uid="{493F8D88-06A7-41E2-A018-CA14671A0EBD}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>